<commit_message>
Added Job Number and Party Bill Feature
</commit_message>
<xml_diff>
--- a/HK/Content/ExcelTemplates/sample-container.xlsx
+++ b/HK/Content/ExcelTemplates/sample-container.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Items" sheetId="2" r:id="rId1"/>
     <sheet name="Container" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="161">
   <si>
     <t>BuyerName</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t>23 CTNS</t>
+  </si>
+  <si>
+    <t>JobNumber</t>
   </si>
 </sst>
 </file>
@@ -547,15 +550,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S74" totalsRowShown="0">
-  <autoFilter ref="A1:S74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:T74" totalsRowShown="0">
+  <autoFilter ref="A1:T74"/>
   <sortState ref="A2:S74">
     <sortCondition ref="A1:A74"/>
   </sortState>
-  <tableColumns count="19">
+  <tableColumns count="20">
     <tableColumn id="1" name="BuyerName"/>
     <tableColumn id="12" name="PartyName"/>
     <tableColumn id="13" name="PartyPhone"/>
+    <tableColumn id="20" name="JobNumber"/>
     <tableColumn id="14" name="BillOnBoardingDate"/>
     <tableColumn id="15" name="BillDeliveryDate"/>
     <tableColumn id="16" name="BillNumber"/>
@@ -862,29 +866,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S74"/>
+  <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="9" width="23.7109375" customWidth="1"/>
-    <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="35.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
-    <col min="16" max="16" width="21" customWidth="1"/>
-    <col min="17" max="17" width="16.85546875" customWidth="1"/>
-    <col min="18" max="18" width="17" customWidth="1"/>
+    <col min="2" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="10" width="23.7109375" customWidth="1"/>
+    <col min="11" max="11" width="27" customWidth="1"/>
+    <col min="12" max="12" width="35.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="14.7109375" customWidth="1"/>
+    <col min="17" max="17" width="21" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1"/>
+    <col min="19" max="19" width="17" customWidth="1"/>
+    <col min="20" max="20" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -895,55 +900,58 @@
         <v>149</v>
       </c>
       <c r="D1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" t="s">
         <v>150</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>151</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>152</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>153</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>155</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>8</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -953,70 +961,73 @@
       <c r="C2">
         <v>204343</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>123</v>
+      </c>
+      <c r="E2" t="s">
         <v>156</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>157</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1023</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>34545</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>158</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>159</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>33</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1200</v>
       </c>
-      <c r="M2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="P2">
+      <c r="N2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
         <v>140</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>56</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>37</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>1800</v>
       </c>
-      <c r="M3" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="P3">
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
         <v>140</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -1026,8 +1037,8 @@
       <c r="C4" t="s">
         <v>88</v>
       </c>
-      <c r="D4" t="s">
-        <v>88</v>
+      <c r="D4">
+        <v>123</v>
       </c>
       <c r="E4" t="s">
         <v>88</v>
@@ -1045,106 +1056,109 @@
         <v>88</v>
       </c>
       <c r="J4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" t="s">
         <v>89</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>90</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>250</v>
       </c>
-      <c r="M4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="P4">
+      <c r="N4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
         <v>112</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>91</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>90</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>260</v>
       </c>
-      <c r="M5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="P5">
+      <c r="N5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
         <v>112</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>88</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>92</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>90</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>180</v>
       </c>
-      <c r="M6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="P6">
+      <c r="N6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>112</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>88</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>93</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>37</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>320</v>
       </c>
-      <c r="M7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="P7">
+      <c r="N7" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
         <v>112</v>
       </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -1154,8 +1168,8 @@
       <c r="C8" t="s">
         <v>107</v>
       </c>
-      <c r="D8" t="s">
-        <v>107</v>
+      <c r="D8">
+        <v>123</v>
       </c>
       <c r="E8" t="s">
         <v>107</v>
@@ -1173,132 +1187,135 @@
         <v>107</v>
       </c>
       <c r="J8" t="s">
+        <v>107</v>
+      </c>
+      <c r="K8" t="s">
         <v>108</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>61</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>580</v>
       </c>
-      <c r="M8" t="s">
-        <v>34</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="P8">
+      <c r="N8" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
         <v>112</v>
       </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>107</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>109</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>61</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>520</v>
       </c>
-      <c r="M9" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="P9">
+      <c r="N9" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
         <v>112</v>
       </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>107</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>110</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>61</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>240</v>
       </c>
-      <c r="M10" t="s">
-        <v>34</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="P10">
+      <c r="N10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
         <v>112</v>
       </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>107</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>111</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>61</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>280</v>
       </c>
-      <c r="M11" t="s">
-        <v>34</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="P11">
+      <c r="N11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
         <v>112</v>
       </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>107</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>112</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>61</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>270</v>
       </c>
-      <c r="M12" t="s">
-        <v>34</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="P12">
+      <c r="N12" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
         <v>112</v>
       </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1327,28 +1344,31 @@
         <v>38</v>
       </c>
       <c r="J13" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" t="s">
         <v>39</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>40</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>617</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>41</v>
       </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="P13">
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
         <v>140</v>
       </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1377,80 +1397,83 @@
         <v>51</v>
       </c>
       <c r="J14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" t="s">
         <v>52</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>50</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>140</v>
       </c>
-      <c r="M14" t="s">
-        <v>34</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="P14">
+      <c r="N14" t="s">
+        <v>34</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
         <v>140</v>
       </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>53</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>50</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>120</v>
       </c>
-      <c r="M15" t="s">
-        <v>34</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="P15">
+      <c r="N15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
         <v>140</v>
       </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>54</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>50</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>140</v>
       </c>
-      <c r="M16" t="s">
-        <v>34</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="P16">
+      <c r="N16" t="s">
+        <v>34</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
         <v>140</v>
       </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -1479,28 +1502,31 @@
         <v>69</v>
       </c>
       <c r="J17" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" t="s">
         <v>70</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>71</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>300</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>48</v>
       </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="P17">
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
         <v>140</v>
       </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -1529,54 +1555,57 @@
         <v>57</v>
       </c>
       <c r="J18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" t="s">
         <v>58</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>59</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>160</v>
       </c>
-      <c r="M18" t="s">
-        <v>34</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="P18">
+      <c r="N18" t="s">
+        <v>34</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
         <v>140</v>
       </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>57</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>60</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>61</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>210</v>
       </c>
-      <c r="M19" t="s">
-        <v>34</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="P19">
+      <c r="N19" t="s">
+        <v>34</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
         <v>140</v>
       </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -1605,132 +1634,135 @@
         <v>72</v>
       </c>
       <c r="J20" t="s">
+        <v>72</v>
+      </c>
+      <c r="K20" t="s">
         <v>75</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>33</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>360</v>
       </c>
-      <c r="M20" t="s">
-        <v>34</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="P20">
+      <c r="N20" t="s">
+        <v>34</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
         <v>140</v>
       </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>72</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>76</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>33</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>300</v>
       </c>
-      <c r="M21" t="s">
-        <v>34</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="P21">
+      <c r="N21" t="s">
+        <v>34</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
         <v>112</v>
       </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>77</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>33</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>300</v>
       </c>
-      <c r="M22" t="s">
-        <v>34</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="P22">
+      <c r="N22" t="s">
+        <v>34</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
         <v>112</v>
       </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>72</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>73</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>37</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>300</v>
       </c>
-      <c r="M23" t="s">
-        <v>34</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="P23">
+      <c r="N23" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
         <v>140</v>
       </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>72</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>74</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>37</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>360</v>
       </c>
-      <c r="M24" t="s">
-        <v>34</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="P24">
+      <c r="N24" t="s">
+        <v>34</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
         <v>140</v>
       </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -1759,28 +1791,31 @@
         <v>67</v>
       </c>
       <c r="J25" t="s">
+        <v>67</v>
+      </c>
+      <c r="K25" t="s">
         <v>68</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>59</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>128</v>
       </c>
-      <c r="M25" t="s">
-        <v>34</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="P25">
+      <c r="N25" t="s">
+        <v>34</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
         <v>140</v>
       </c>
-      <c r="S25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1809,80 +1844,83 @@
         <v>44</v>
       </c>
       <c r="J26" t="s">
+        <v>44</v>
+      </c>
+      <c r="K26" t="s">
         <v>49</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>50</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>250</v>
       </c>
-      <c r="M26" t="s">
-        <v>34</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="P26">
+      <c r="N26" t="s">
+        <v>34</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
         <v>140</v>
       </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>45</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>19</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>120</v>
       </c>
-      <c r="M27" t="s">
-        <v>34</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="P27">
+      <c r="N27" t="s">
+        <v>34</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
         <v>140</v>
       </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>44</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>46</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>47</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>340</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>48</v>
       </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-      <c r="P28">
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
         <v>140</v>
       </c>
-      <c r="S28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>113</v>
       </c>
@@ -1911,106 +1949,109 @@
         <v>113</v>
       </c>
       <c r="J29" t="s">
+        <v>113</v>
+      </c>
+      <c r="K29" t="s">
         <v>114</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>19</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>12</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>14</v>
       </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="P29">
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
         <v>112</v>
       </c>
-      <c r="S29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>113</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>115</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>19</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>90</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>14</v>
       </c>
-      <c r="N30">
-        <v>0</v>
-      </c>
-      <c r="P30">
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
         <v>112</v>
       </c>
-      <c r="S30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>113</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>116</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>19</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>144</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>14</v>
       </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="P31">
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
         <v>112</v>
       </c>
-      <c r="S31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>113</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>117</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>19</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>12</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>14</v>
       </c>
-      <c r="N32">
-        <v>0</v>
-      </c>
-      <c r="P32">
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
         <v>112</v>
       </c>
-      <c r="S32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -2039,28 +2080,31 @@
         <v>65</v>
       </c>
       <c r="J33" t="s">
+        <v>65</v>
+      </c>
+      <c r="K33" t="s">
         <v>66</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>59</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <v>128</v>
       </c>
-      <c r="M33" t="s">
-        <v>34</v>
-      </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-      <c r="P33">
+      <c r="N33" t="s">
+        <v>34</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
         <v>140</v>
       </c>
-      <c r="S33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -2088,52 +2132,55 @@
       <c r="I34" t="s">
         <v>78</v>
       </c>
-      <c r="K34" t="s">
+      <c r="J34" t="s">
+        <v>78</v>
+      </c>
+      <c r="L34" t="s">
         <v>36</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <v>600</v>
       </c>
-      <c r="M34" t="s">
-        <v>34</v>
-      </c>
-      <c r="N34">
-        <v>0</v>
-      </c>
-      <c r="P34">
+      <c r="N34" t="s">
+        <v>34</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
         <v>112</v>
       </c>
-      <c r="S34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>78</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>79</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>37</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <v>1200</v>
       </c>
-      <c r="M35" t="s">
-        <v>34</v>
-      </c>
-      <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="P35">
+      <c r="N35" t="s">
+        <v>34</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
         <v>112</v>
       </c>
-      <c r="S35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -2162,155 +2209,158 @@
         <v>80</v>
       </c>
       <c r="J36" t="s">
+        <v>80</v>
+      </c>
+      <c r="K36" t="s">
         <v>87</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>61</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>120</v>
       </c>
-      <c r="M36" t="s">
-        <v>34</v>
-      </c>
-      <c r="N36">
-        <v>0</v>
-      </c>
-      <c r="P36">
+      <c r="N36" t="s">
+        <v>34</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
         <v>112</v>
       </c>
-      <c r="S36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>80</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>85</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>86</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>480</v>
       </c>
-      <c r="M37" t="s">
-        <v>34</v>
-      </c>
-      <c r="N37">
-        <v>0</v>
-      </c>
-      <c r="P37">
+      <c r="N37" t="s">
+        <v>34</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
         <v>112</v>
       </c>
-      <c r="S37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>80</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
         <v>81</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>82</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <v>208</v>
       </c>
-      <c r="M38" t="s">
-        <v>34</v>
-      </c>
-      <c r="N38">
-        <v>0</v>
-      </c>
-      <c r="P38">
+      <c r="N38" t="s">
+        <v>34</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
         <v>112</v>
       </c>
-      <c r="S38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>80</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>83</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>82</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <v>300</v>
       </c>
-      <c r="M39" t="s">
-        <v>34</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-      <c r="P39">
+      <c r="N39" t="s">
+        <v>34</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
         <v>112</v>
       </c>
-      <c r="S39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>80</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>84</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>50</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <v>250</v>
       </c>
-      <c r="M40" t="s">
-        <v>34</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="P40">
+      <c r="N40" t="s">
+        <v>34</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
         <v>112</v>
       </c>
-      <c r="S40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>80</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>50</v>
       </c>
-      <c r="L41">
+      <c r="M41">
         <v>240</v>
       </c>
-      <c r="M41" t="s">
-        <v>34</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="P41">
+      <c r="N41" t="s">
+        <v>34</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
         <v>112</v>
       </c>
-      <c r="S41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -2339,54 +2389,57 @@
         <v>62</v>
       </c>
       <c r="J42" t="s">
+        <v>62</v>
+      </c>
+      <c r="K42" t="s">
         <v>63</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>59</v>
       </c>
-      <c r="L42">
+      <c r="M42">
         <v>160</v>
       </c>
-      <c r="M42" t="s">
-        <v>34</v>
-      </c>
-      <c r="N42">
-        <v>0</v>
-      </c>
-      <c r="P42">
+      <c r="N42" t="s">
+        <v>34</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
         <v>140</v>
       </c>
-      <c r="S42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>62</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>64</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>61</v>
       </c>
-      <c r="L43">
+      <c r="M43">
         <v>210</v>
       </c>
-      <c r="M43" t="s">
-        <v>34</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
-      </c>
-      <c r="P43">
+      <c r="N43" t="s">
+        <v>34</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
         <v>140</v>
       </c>
-      <c r="S43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -2415,392 +2468,395 @@
         <v>11</v>
       </c>
       <c r="J44" t="s">
+        <v>11</v>
+      </c>
+      <c r="K44" t="s">
         <v>12</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>13</v>
       </c>
-      <c r="L44">
+      <c r="M44">
         <v>120</v>
       </c>
-      <c r="M44" t="s">
+      <c r="N44" t="s">
         <v>14</v>
       </c>
-      <c r="N44">
-        <v>0</v>
-      </c>
-      <c r="P44">
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
         <v>120</v>
       </c>
-      <c r="S44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
-      <c r="J45" t="s">
+      <c r="K45" t="s">
         <v>15</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
         <v>13</v>
       </c>
-      <c r="L45">
+      <c r="M45">
         <v>90</v>
       </c>
-      <c r="M45" t="s">
+      <c r="N45" t="s">
         <v>14</v>
       </c>
-      <c r="N45">
-        <v>0</v>
-      </c>
-      <c r="P45">
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
         <v>120</v>
       </c>
-      <c r="S45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>11</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>20</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
         <v>13</v>
       </c>
-      <c r="L46">
+      <c r="M46">
         <v>120</v>
       </c>
-      <c r="M46" t="s">
+      <c r="N46" t="s">
         <v>14</v>
       </c>
-      <c r="N46">
-        <v>0</v>
-      </c>
-      <c r="P46">
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
         <v>120</v>
       </c>
-      <c r="S46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>11</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>22</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
         <v>13</v>
       </c>
-      <c r="L47">
+      <c r="M47">
         <v>90</v>
       </c>
-      <c r="M47" t="s">
+      <c r="N47" t="s">
         <v>14</v>
       </c>
-      <c r="N47">
-        <v>0</v>
-      </c>
-      <c r="P47">
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
         <v>120</v>
       </c>
-      <c r="S47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>11</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>24</v>
       </c>
-      <c r="K48" t="s">
+      <c r="L48" t="s">
         <v>13</v>
       </c>
-      <c r="L48">
+      <c r="M48">
         <v>120</v>
       </c>
-      <c r="M48" t="s">
+      <c r="N48" t="s">
         <v>14</v>
       </c>
-      <c r="N48">
-        <v>0</v>
-      </c>
-      <c r="P48">
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="Q48">
         <v>120</v>
       </c>
-      <c r="S48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>11</v>
       </c>
-      <c r="J49" t="s">
+      <c r="K49" t="s">
         <v>16</v>
       </c>
-      <c r="K49" t="s">
+      <c r="L49" t="s">
         <v>17</v>
       </c>
-      <c r="L49">
+      <c r="M49">
         <v>60</v>
       </c>
-      <c r="M49" t="s">
+      <c r="N49" t="s">
         <v>14</v>
       </c>
-      <c r="N49">
-        <v>0</v>
-      </c>
-      <c r="P49">
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
         <v>120</v>
       </c>
-      <c r="S49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>11</v>
       </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>23</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>17</v>
       </c>
-      <c r="L50">
+      <c r="M50">
         <v>60</v>
       </c>
-      <c r="M50" t="s">
+      <c r="N50" t="s">
         <v>14</v>
       </c>
-      <c r="N50">
-        <v>0</v>
-      </c>
-      <c r="P50">
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
         <v>120</v>
       </c>
-      <c r="S50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>11</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>25</v>
       </c>
-      <c r="K51" t="s">
+      <c r="L51" t="s">
         <v>17</v>
       </c>
-      <c r="L51">
+      <c r="M51">
         <v>60</v>
       </c>
-      <c r="M51" t="s">
+      <c r="N51" t="s">
         <v>14</v>
       </c>
-      <c r="N51">
-        <v>0</v>
-      </c>
-      <c r="P51">
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
         <v>120</v>
       </c>
-      <c r="S51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>11</v>
       </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>18</v>
       </c>
-      <c r="K52" t="s">
+      <c r="L52" t="s">
         <v>19</v>
       </c>
-      <c r="L52">
+      <c r="M52">
         <v>120</v>
       </c>
-      <c r="M52" t="s">
+      <c r="N52" t="s">
         <v>14</v>
       </c>
-      <c r="N52">
-        <v>0</v>
-      </c>
-      <c r="P52">
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="Q52">
         <v>120</v>
       </c>
-      <c r="S52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
-      <c r="J53" t="s">
+      <c r="K53" t="s">
         <v>21</v>
       </c>
-      <c r="K53" t="s">
+      <c r="L53" t="s">
         <v>19</v>
       </c>
-      <c r="L53">
+      <c r="M53">
         <v>120</v>
       </c>
-      <c r="M53" t="s">
+      <c r="N53" t="s">
         <v>14</v>
       </c>
-      <c r="N53">
-        <v>0</v>
-      </c>
-      <c r="P53">
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
         <v>120</v>
       </c>
-      <c r="S53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>11</v>
       </c>
-      <c r="J54" t="s">
+      <c r="K54" t="s">
         <v>26</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" t="s">
         <v>19</v>
       </c>
-      <c r="L54">
+      <c r="M54">
         <v>60</v>
       </c>
-      <c r="M54" t="s">
+      <c r="N54" t="s">
         <v>14</v>
       </c>
-      <c r="N54">
-        <v>0</v>
-      </c>
-      <c r="P54">
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="Q54">
         <v>120</v>
       </c>
-      <c r="S54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>11</v>
       </c>
-      <c r="J55" t="s">
+      <c r="K55" t="s">
         <v>27</v>
       </c>
-      <c r="K55" t="s">
+      <c r="L55" t="s">
         <v>19</v>
       </c>
-      <c r="L55">
+      <c r="M55">
         <v>156</v>
       </c>
-      <c r="M55" t="s">
+      <c r="N55" t="s">
         <v>14</v>
       </c>
-      <c r="N55">
-        <v>0</v>
-      </c>
-      <c r="P55">
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="Q55">
         <v>120</v>
       </c>
-      <c r="S55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>11</v>
       </c>
-      <c r="J56" t="s">
+      <c r="K56" t="s">
         <v>28</v>
       </c>
-      <c r="K56" t="s">
+      <c r="L56" t="s">
         <v>19</v>
       </c>
-      <c r="L56">
+      <c r="M56">
         <v>162</v>
       </c>
-      <c r="M56" t="s">
+      <c r="N56" t="s">
         <v>14</v>
       </c>
-      <c r="N56">
-        <v>0</v>
-      </c>
-      <c r="P56">
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="Q56">
         <v>120</v>
       </c>
-      <c r="S56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>11</v>
       </c>
-      <c r="J57" t="s">
+      <c r="K57" t="s">
         <v>29</v>
       </c>
-      <c r="K57" t="s">
+      <c r="L57" t="s">
         <v>19</v>
       </c>
-      <c r="L57">
+      <c r="M57">
         <v>60</v>
       </c>
-      <c r="M57" t="s">
+      <c r="N57" t="s">
         <v>14</v>
       </c>
-      <c r="N57">
-        <v>0</v>
-      </c>
-      <c r="P57">
+      <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="Q57">
         <v>120</v>
       </c>
-      <c r="S57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>11</v>
       </c>
-      <c r="J58" t="s">
+      <c r="K58" t="s">
         <v>30</v>
       </c>
-      <c r="K58" t="s">
+      <c r="L58" t="s">
         <v>19</v>
       </c>
-      <c r="L58">
+      <c r="M58">
         <v>60</v>
       </c>
-      <c r="M58" t="s">
+      <c r="N58" t="s">
         <v>14</v>
       </c>
-      <c r="N58">
-        <v>0</v>
-      </c>
-      <c r="P58">
+      <c r="O58">
+        <v>0</v>
+      </c>
+      <c r="Q58">
         <v>140</v>
       </c>
-      <c r="S58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -2828,274 +2884,277 @@
       <c r="I59" t="s">
         <v>94</v>
       </c>
-      <c r="K59" t="s">
+      <c r="J59" t="s">
+        <v>94</v>
+      </c>
+      <c r="L59" t="s">
         <v>106</v>
       </c>
-      <c r="L59">
+      <c r="M59">
         <v>17</v>
       </c>
-      <c r="M59" t="s">
+      <c r="N59" t="s">
         <v>48</v>
       </c>
-      <c r="N59">
-        <v>0</v>
-      </c>
-      <c r="P59">
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
         <v>112</v>
       </c>
-      <c r="S59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>94</v>
       </c>
-      <c r="K60" t="s">
+      <c r="L60" t="s">
         <v>101</v>
       </c>
-      <c r="L60">
+      <c r="M60">
         <v>3</v>
       </c>
-      <c r="M60" t="s">
+      <c r="N60" t="s">
         <v>48</v>
       </c>
-      <c r="N60">
-        <v>0</v>
-      </c>
-      <c r="P60">
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="Q60">
         <v>112</v>
       </c>
-      <c r="S60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>94</v>
       </c>
-      <c r="K61" t="s">
+      <c r="L61" t="s">
         <v>101</v>
       </c>
-      <c r="L61">
+      <c r="M61">
         <v>51</v>
       </c>
-      <c r="M61" t="s">
-        <v>34</v>
-      </c>
-      <c r="N61">
-        <v>0</v>
-      </c>
-      <c r="P61">
+      <c r="N61" t="s">
+        <v>34</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="Q61">
         <v>112</v>
       </c>
-      <c r="S61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>94</v>
       </c>
-      <c r="K62" t="s">
+      <c r="L62" t="s">
         <v>99</v>
       </c>
-      <c r="L62">
+      <c r="M62">
         <v>5</v>
       </c>
-      <c r="M62" t="s">
+      <c r="N62" t="s">
         <v>48</v>
       </c>
-      <c r="N62">
-        <v>0</v>
-      </c>
-      <c r="P62">
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="Q62">
         <v>112</v>
       </c>
-      <c r="S62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>94</v>
       </c>
-      <c r="J63" t="s">
+      <c r="K63" t="s">
         <v>95</v>
       </c>
-      <c r="K63" t="s">
+      <c r="L63" t="s">
         <v>13</v>
       </c>
-      <c r="L63">
+      <c r="M63">
         <v>10</v>
       </c>
-      <c r="M63" t="s">
+      <c r="N63" t="s">
         <v>48</v>
       </c>
-      <c r="N63">
-        <v>0</v>
-      </c>
-      <c r="P63">
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
         <v>112</v>
       </c>
-      <c r="S63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>94</v>
       </c>
-      <c r="J64" t="s">
+      <c r="K64" t="s">
         <v>104</v>
       </c>
-      <c r="K64" t="s">
+      <c r="L64" t="s">
         <v>105</v>
       </c>
-      <c r="L64">
+      <c r="M64">
         <v>48</v>
       </c>
-      <c r="M64" t="s">
-        <v>34</v>
-      </c>
-      <c r="N64">
-        <v>0</v>
-      </c>
-      <c r="P64">
+      <c r="N64" t="s">
+        <v>34</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
+      <c r="Q64">
         <v>112</v>
       </c>
-      <c r="S64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>94</v>
       </c>
-      <c r="K65" t="s">
+      <c r="L65" t="s">
         <v>100</v>
       </c>
-      <c r="L65">
+      <c r="M65">
         <v>7</v>
       </c>
-      <c r="M65" t="s">
+      <c r="N65" t="s">
         <v>48</v>
       </c>
-      <c r="N65">
-        <v>0</v>
-      </c>
-      <c r="P65">
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="Q65">
         <v>112</v>
       </c>
-      <c r="S65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>94</v>
       </c>
-      <c r="J66" t="s">
+      <c r="K66" t="s">
         <v>103</v>
       </c>
-      <c r="K66" t="s">
+      <c r="L66" t="s">
         <v>100</v>
       </c>
-      <c r="L66">
+      <c r="M66">
         <v>13</v>
       </c>
-      <c r="M66" t="s">
+      <c r="N66" t="s">
         <v>48</v>
       </c>
-      <c r="N66">
-        <v>0</v>
-      </c>
-      <c r="P66">
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
         <v>112</v>
       </c>
-      <c r="S66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>94</v>
       </c>
-      <c r="J67" t="s">
+      <c r="K67" t="s">
         <v>96</v>
       </c>
-      <c r="K67" t="s">
+      <c r="L67" t="s">
         <v>97</v>
       </c>
-      <c r="L67">
+      <c r="M67">
         <v>8</v>
       </c>
-      <c r="M67" t="s">
+      <c r="N67" t="s">
         <v>48</v>
       </c>
-      <c r="N67">
-        <v>0</v>
-      </c>
-      <c r="P67">
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="Q67">
         <v>112</v>
       </c>
-      <c r="S67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>94</v>
       </c>
-      <c r="J68" t="s">
+      <c r="K68" t="s">
         <v>98</v>
       </c>
-      <c r="K68" t="s">
+      <c r="L68" t="s">
         <v>97</v>
       </c>
-      <c r="L68">
+      <c r="M68">
         <v>6</v>
       </c>
-      <c r="M68" t="s">
+      <c r="N68" t="s">
         <v>48</v>
       </c>
-      <c r="N68">
-        <v>0</v>
-      </c>
-      <c r="P68">
+      <c r="O68">
+        <v>0</v>
+      </c>
+      <c r="Q68">
         <v>112</v>
       </c>
-      <c r="S68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>94</v>
       </c>
-      <c r="J69" t="s">
+      <c r="K69" t="s">
         <v>102</v>
       </c>
-      <c r="K69" t="s">
+      <c r="L69" t="s">
         <v>97</v>
       </c>
-      <c r="L69">
+      <c r="M69">
         <v>14</v>
       </c>
-      <c r="M69" t="s">
+      <c r="N69" t="s">
         <v>48</v>
       </c>
-      <c r="N69">
-        <v>0</v>
-      </c>
-      <c r="P69">
+      <c r="O69">
+        <v>0</v>
+      </c>
+      <c r="Q69">
         <v>112</v>
       </c>
-      <c r="S69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>31</v>
       </c>
@@ -3124,77 +3183,80 @@
         <v>31</v>
       </c>
       <c r="J70" t="s">
+        <v>31</v>
+      </c>
+      <c r="K70" t="s">
         <v>35</v>
       </c>
-      <c r="K70" t="s">
+      <c r="L70" t="s">
         <v>36</v>
       </c>
-      <c r="L70">
+      <c r="M70">
         <v>1000</v>
       </c>
-      <c r="M70" t="s">
-        <v>34</v>
-      </c>
-      <c r="N70">
-        <v>0</v>
-      </c>
-      <c r="P70">
+      <c r="N70" t="s">
+        <v>34</v>
+      </c>
+      <c r="O70">
+        <v>0</v>
+      </c>
+      <c r="Q70">
         <v>140</v>
       </c>
-      <c r="S70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>31</v>
       </c>
-      <c r="J71" t="s">
+      <c r="K71" t="s">
         <v>32</v>
       </c>
-      <c r="K71" t="s">
+      <c r="L71" t="s">
         <v>33</v>
       </c>
-      <c r="L71">
+      <c r="M71">
         <v>600</v>
       </c>
-      <c r="M71" t="s">
-        <v>34</v>
-      </c>
-      <c r="N71">
-        <v>0</v>
-      </c>
-      <c r="P71">
+      <c r="N71" t="s">
+        <v>34</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
         <v>140</v>
       </c>
-      <c r="S71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>31</v>
       </c>
-      <c r="K72" t="s">
+      <c r="L72" t="s">
         <v>37</v>
       </c>
-      <c r="L72">
+      <c r="M72">
         <v>500</v>
       </c>
-      <c r="M72" t="s">
-        <v>34</v>
-      </c>
-      <c r="N72">
-        <v>0</v>
-      </c>
-      <c r="P72">
+      <c r="N72" t="s">
+        <v>34</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
+      </c>
+      <c r="Q72">
         <v>140</v>
       </c>
-      <c r="S72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>42</v>
       </c>
@@ -3223,47 +3285,50 @@
         <v>42</v>
       </c>
       <c r="J73" t="s">
+        <v>42</v>
+      </c>
+      <c r="K73" t="s">
         <v>43</v>
       </c>
-      <c r="K73" t="s">
+      <c r="L73" t="s">
         <v>36</v>
       </c>
-      <c r="L73">
+      <c r="M73">
         <v>1200</v>
       </c>
-      <c r="M73" t="s">
-        <v>34</v>
-      </c>
-      <c r="N73">
-        <v>0</v>
-      </c>
-      <c r="P73">
+      <c r="N73" t="s">
+        <v>34</v>
+      </c>
+      <c r="O73">
+        <v>0</v>
+      </c>
+      <c r="Q73">
         <v>140</v>
       </c>
-      <c r="S73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>42</v>
       </c>
-      <c r="K74" t="s">
+      <c r="L74" t="s">
         <v>37</v>
       </c>
-      <c r="L74">
+      <c r="M74">
         <v>600</v>
       </c>
-      <c r="M74" t="s">
-        <v>34</v>
-      </c>
-      <c r="N74">
-        <v>0</v>
-      </c>
-      <c r="P74">
+      <c r="N74" t="s">
+        <v>34</v>
+      </c>
+      <c r="O74">
+        <v>0</v>
+      </c>
+      <c r="Q74">
         <v>140</v>
       </c>
-      <c r="S74">
+      <c r="T74">
         <v>0</v>
       </c>
     </row>

</xml_diff>